<commit_message>
new: PSFB PCB rev. 1.0 hotfix
</commit_message>
<xml_diff>
--- a/PSFB/Hardware/ProductionFiles/assembly/CP_Inverter_BOM.xlsx
+++ b/PSFB/Hardware/ProductionFiles/assembly/CP_Inverter_BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\work\CP_Inverter\PSFB\Hardware\ProductionFiles\assembly\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86ECFCCB-75CA-4923-96BD-5A7FE0549FCF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79420654-63A3-4E08-8CA2-3037F12BAE9B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="277">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="279">
   <si>
     <t>PartNumber</t>
   </si>
@@ -235,9 +235,6 @@
     <t>Isolated Module DC DC Converter 1 Output 24V 42mA 21.6V - 26.4V Input</t>
   </si>
   <si>
-    <t>https://www.chipdip.ru/product/b0505s-1wr2</t>
-  </si>
-  <si>
     <t>D4, D10, D12, D14</t>
   </si>
   <si>
@@ -598,9 +595,6 @@
     <t>B66398W1024T001</t>
   </si>
   <si>
-    <t>N97 B66397G0000X197 сore / B66398W1024T001 coil former</t>
-  </si>
-  <si>
     <t>https://www.digikey.com/en/products/detail/epcos-tdk-electronics/B66398W1024T001/3914904</t>
   </si>
   <si>
@@ -857,6 +851,18 @@
   </si>
   <si>
     <t>https://www.digikey.com/en/products/detail/te-connectivity-amp-connectors/6PCV-02-006/1277933</t>
+  </si>
+  <si>
+    <t>8853522130111</t>
+  </si>
+  <si>
+    <t>60311002111526</t>
+  </si>
+  <si>
+    <t>N97 B66397G0000X197 сore / B66398W1024T001 coil former, DNP</t>
+  </si>
+  <si>
+    <t>https://lcsc.com/product-detail/Power-Modules_MORNSUN-Guangzhou-S-T-B2424S-1WR2_C91799.html</t>
   </si>
 </sst>
 </file>
@@ -978,7 +984,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1013,32 +1019,11 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1052,11 +1037,26 @@
     <xf numFmtId="49" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1342,43 +1342,43 @@
   <dimension ref="A1:I64"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J25" sqref="J25"/>
+      <selection activeCell="H17" sqref="H17:I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="18.45" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="62.921875" style="21" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.921875" style="22" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="32.4609375" style="22" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.15234375" style="23" customWidth="1"/>
-    <col min="5" max="5" width="11.07421875" style="21" customWidth="1"/>
-    <col min="6" max="6" width="67.921875" style="21" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.23046875" style="16" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.15234375" style="21"/>
+    <col min="1" max="1" width="62.921875" style="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.921875" style="15" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32.4609375" style="15" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.15234375" style="16" customWidth="1"/>
+    <col min="5" max="5" width="11.07421875" style="14" customWidth="1"/>
+    <col min="6" max="6" width="67.921875" style="14" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.23046875" style="13" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.15234375" style="14"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.5">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="24" t="s">
+      <c r="C1" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="25" t="s">
+      <c r="D1" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="24" t="s">
+      <c r="E1" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="24" t="s">
+      <c r="F1" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
-      <c r="I1" s="16"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="13"/>
     </row>
     <row r="2" spans="1:9" ht="73.75" x14ac:dyDescent="0.5">
       <c r="A2" s="1" t="s">
@@ -1400,8 +1400,8 @@
         <v>10</v>
       </c>
       <c r="G2" s="10"/>
-      <c r="H2" s="16"/>
-      <c r="I2" s="16"/>
+      <c r="H2" s="13"/>
+      <c r="I2" s="13"/>
     </row>
     <row r="3" spans="1:9" ht="55.3" x14ac:dyDescent="0.5">
       <c r="A3" s="1" t="s">
@@ -1423,8 +1423,8 @@
         <v>15</v>
       </c>
       <c r="G3" s="10"/>
-      <c r="H3" s="16"/>
-      <c r="I3" s="16"/>
+      <c r="H3" s="13"/>
+      <c r="I3" s="13"/>
     </row>
     <row r="4" spans="1:9" ht="55.3" x14ac:dyDescent="0.5">
       <c r="A4" s="1" t="s">
@@ -1446,8 +1446,8 @@
         <v>19</v>
       </c>
       <c r="G4" s="10"/>
-      <c r="H4" s="16"/>
-      <c r="I4" s="16"/>
+      <c r="H4" s="13"/>
+      <c r="I4" s="13"/>
     </row>
     <row r="5" spans="1:9" ht="73.75" x14ac:dyDescent="0.5">
       <c r="A5" s="1" t="s">
@@ -1537,8 +1537,8 @@
       <c r="A9" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B9" s="2">
-        <v>8853522130111</v>
+      <c r="B9" s="2" t="s">
+        <v>275</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>40</v>
@@ -1549,7 +1549,7 @@
       <c r="E9" s="2">
         <v>1</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="F9" s="5" t="s">
         <v>42</v>
       </c>
       <c r="G9" s="10"/>
@@ -1650,7 +1650,7 @@
       <c r="E14" s="2">
         <v>1</v>
       </c>
-      <c r="F14" s="1" t="s">
+      <c r="F14" s="5" t="s">
         <v>65</v>
       </c>
       <c r="G14" s="10"/>
@@ -1670,981 +1670,985 @@
         <v>4</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>69</v>
+        <v>278</v>
       </c>
       <c r="G15" s="10"/>
     </row>
     <row r="16" spans="1:9" ht="55.3" x14ac:dyDescent="0.5">
       <c r="A16" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B16" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="C16" s="2" t="s">
         <v>71</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>72</v>
       </c>
       <c r="D16" s="2"/>
       <c r="E16" s="2">
         <v>4</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G16" s="10"/>
     </row>
     <row r="17" spans="1:7" ht="55.3" x14ac:dyDescent="0.5">
       <c r="A17" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B17" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="C17" s="2" t="s">
         <v>75</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>76</v>
       </c>
       <c r="D17" s="2"/>
       <c r="E17" s="2">
         <v>1</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G17" s="10"/>
     </row>
     <row r="18" spans="1:7" ht="55.3" x14ac:dyDescent="0.5">
       <c r="A18" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B18" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="C18" s="4" t="s">
         <v>79</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>80</v>
       </c>
       <c r="D18" s="4"/>
       <c r="E18" s="4">
         <v>2</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G18" s="10"/>
     </row>
     <row r="19" spans="1:7" ht="55.3" x14ac:dyDescent="0.5">
       <c r="A19" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="B19" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="B19" s="4" t="s">
+      <c r="C19" s="4" t="s">
         <v>83</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>84</v>
       </c>
       <c r="D19" s="4"/>
       <c r="E19" s="4">
         <v>1</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G19" s="10"/>
     </row>
     <row r="20" spans="1:7" ht="55.3" x14ac:dyDescent="0.5">
       <c r="A20" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="B20" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="B20" s="4" t="s">
+      <c r="C20" s="4" t="s">
         <v>87</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>88</v>
       </c>
       <c r="D20" s="4"/>
       <c r="E20" s="4">
         <v>1</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G20" s="10"/>
     </row>
     <row r="21" spans="1:7" ht="55.3" x14ac:dyDescent="0.5">
       <c r="A21" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="B21" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="B21" s="4" t="s">
-        <v>91</v>
-      </c>
       <c r="C21" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D21" s="4"/>
       <c r="E21" s="4">
         <v>1</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G21" s="10"/>
     </row>
     <row r="22" spans="1:7" ht="73.75" x14ac:dyDescent="0.5">
       <c r="A22" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="B22" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="B22" s="4" t="s">
+      <c r="C22" s="4" t="s">
         <v>94</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>95</v>
       </c>
       <c r="D22" s="4"/>
       <c r="E22" s="4">
         <v>1</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G22" s="10"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A23" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="B23" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="B23" s="4" t="s">
+      <c r="C23" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="C23" s="4" t="s">
+      <c r="D23" s="4" t="s">
         <v>99</v>
-      </c>
-      <c r="D23" s="4" t="s">
-        <v>100</v>
       </c>
       <c r="E23" s="4">
         <v>1</v>
       </c>
-      <c r="F23" s="26" t="s">
-        <v>101</v>
+      <c r="F23" s="18" t="s">
+        <v>100</v>
       </c>
       <c r="G23" s="10"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A24" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="B24" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="B24" s="4" t="s">
-        <v>103</v>
-      </c>
       <c r="C24" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="D24" s="4" t="s">
         <v>99</v>
-      </c>
-      <c r="D24" s="4" t="s">
-        <v>100</v>
       </c>
       <c r="E24" s="4">
         <v>1</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G24" s="10"/>
     </row>
     <row r="25" spans="1:7" ht="55.3" x14ac:dyDescent="0.5">
       <c r="A25" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="B25" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="B25" s="4" t="s">
+      <c r="C25" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="C25" s="4" t="s">
+      <c r="D25" s="4" t="s">
         <v>107</v>
-      </c>
-      <c r="D25" s="4" t="s">
-        <v>108</v>
       </c>
       <c r="E25" s="4">
         <v>1</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G25" s="10"/>
     </row>
     <row r="26" spans="1:7" ht="73.75" x14ac:dyDescent="0.5">
       <c r="A26" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="B26" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="B26" s="4" t="s">
+      <c r="C26" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="C26" s="4" t="s">
+      <c r="D26" s="4" t="s">
         <v>112</v>
-      </c>
-      <c r="D26" s="4" t="s">
-        <v>113</v>
       </c>
       <c r="E26" s="4">
         <v>6</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G26" s="10"/>
     </row>
     <row r="27" spans="1:7" ht="73.75" x14ac:dyDescent="0.5">
       <c r="A27" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="B27" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="B27" s="4" t="s">
+      <c r="C27" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="C27" s="4" t="s">
+      <c r="D27" s="4" t="s">
         <v>117</v>
-      </c>
-      <c r="D27" s="4" t="s">
-        <v>118</v>
       </c>
       <c r="E27" s="4">
         <v>4</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G27" s="10"/>
     </row>
     <row r="28" spans="1:7" ht="55.3" x14ac:dyDescent="0.5">
       <c r="A28" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="B28" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="B28" s="4" t="s">
+      <c r="C28" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="C28" s="4" t="s">
+      <c r="D28" s="4" t="s">
         <v>122</v>
-      </c>
-      <c r="D28" s="4" t="s">
-        <v>123</v>
       </c>
       <c r="E28" s="4">
         <v>1</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G28" s="10"/>
     </row>
     <row r="29" spans="1:7" ht="55.3" x14ac:dyDescent="0.5">
       <c r="A29" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B29" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="B29" s="2" t="s">
+      <c r="C29" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="C29" s="2" t="s">
+      <c r="D29" s="2" t="s">
         <v>127</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>128</v>
       </c>
       <c r="E29" s="2">
         <v>4</v>
       </c>
       <c r="F29" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G29" s="10"/>
     </row>
     <row r="30" spans="1:7" ht="73.75" x14ac:dyDescent="0.5">
       <c r="A30" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B30" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="B30" s="2" t="s">
+      <c r="C30" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="C30" s="2" t="s">
+      <c r="D30" s="2" t="s">
         <v>132</v>
-      </c>
-      <c r="D30" s="2" t="s">
-        <v>133</v>
       </c>
       <c r="E30" s="2">
         <v>22</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="G30" s="15"/>
+        <v>133</v>
+      </c>
+      <c r="G30" s="12"/>
     </row>
     <row r="31" spans="1:7" ht="73.75" x14ac:dyDescent="0.5">
       <c r="A31" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="B31" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="B31" s="4" t="s">
+      <c r="C31" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="C31" s="4" t="s">
+      <c r="D31" s="4" t="s">
         <v>137</v>
-      </c>
-      <c r="D31" s="4" t="s">
-        <v>138</v>
       </c>
       <c r="E31" s="4">
         <v>12</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="G31" s="10"/>
     </row>
     <row r="32" spans="1:7" ht="73.75" x14ac:dyDescent="0.5">
       <c r="A32" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="B32" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="B32" s="4" t="s">
+      <c r="C32" s="4" t="s">
         <v>141</v>
       </c>
-      <c r="C32" s="4" t="s">
+      <c r="D32" s="4" t="s">
         <v>142</v>
-      </c>
-      <c r="D32" s="4" t="s">
-        <v>143</v>
       </c>
       <c r="E32" s="4">
         <v>22</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G32" s="10"/>
     </row>
     <row r="33" spans="1:7" ht="92.15" x14ac:dyDescent="0.5">
       <c r="A33" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="B33" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="B33" s="4" t="s">
+      <c r="C33" s="4" t="s">
         <v>146</v>
       </c>
-      <c r="C33" s="4" t="s">
+      <c r="D33" s="4" t="s">
         <v>147</v>
-      </c>
-      <c r="D33" s="4" t="s">
-        <v>148</v>
       </c>
       <c r="E33" s="4">
         <v>8</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="G33" s="10"/>
     </row>
     <row r="34" spans="1:7" ht="73.75" x14ac:dyDescent="0.5">
       <c r="A34" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="B34" s="4" t="s">
         <v>150</v>
       </c>
-      <c r="B34" s="4" t="s">
+      <c r="C34" s="4" t="s">
         <v>151</v>
       </c>
-      <c r="C34" s="4" t="s">
+      <c r="D34" s="4" t="s">
         <v>152</v>
-      </c>
-      <c r="D34" s="4" t="s">
-        <v>153</v>
       </c>
       <c r="E34" s="4">
         <v>3</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="G34" s="10"/>
     </row>
     <row r="35" spans="1:7" ht="55.3" x14ac:dyDescent="0.5">
       <c r="A35" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="B35" s="4" t="s">
         <v>155</v>
       </c>
-      <c r="B35" s="4" t="s">
+      <c r="C35" s="4" t="s">
         <v>156</v>
       </c>
-      <c r="C35" s="4" t="s">
+      <c r="D35" s="4" t="s">
         <v>157</v>
-      </c>
-      <c r="D35" s="4" t="s">
-        <v>158</v>
       </c>
       <c r="E35" s="4">
         <v>3</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="G35" s="10"/>
     </row>
     <row r="36" spans="1:7" ht="73.75" x14ac:dyDescent="0.5">
       <c r="A36" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="B36" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="B36" s="2" t="s">
+      <c r="C36" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="C36" s="2" t="s">
+      <c r="D36" s="2" t="s">
         <v>162</v>
-      </c>
-      <c r="D36" s="2" t="s">
-        <v>163</v>
       </c>
       <c r="E36" s="2">
         <v>1</v>
       </c>
       <c r="F36" s="5" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="G36" s="10"/>
     </row>
     <row r="37" spans="1:7" ht="73.75" x14ac:dyDescent="0.5">
       <c r="A37" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="B37" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="B37" s="2" t="s">
+      <c r="C37" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="C37" s="2" t="s">
+      <c r="D37" s="2" t="s">
         <v>167</v>
-      </c>
-      <c r="D37" s="2" t="s">
-        <v>168</v>
       </c>
       <c r="E37" s="2">
         <v>1</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="G37" s="10"/>
     </row>
     <row r="38" spans="1:7" ht="92.15" x14ac:dyDescent="0.5">
       <c r="A38" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="B38" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="B38" s="2" t="s">
+      <c r="C38" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="C38" s="2" t="s">
-        <v>172</v>
-      </c>
       <c r="D38" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E38" s="2">
         <v>2</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="G38" s="10"/>
     </row>
     <row r="39" spans="1:7" ht="73.75" x14ac:dyDescent="0.5">
       <c r="A39" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="B39" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="B39" s="2" t="s">
+      <c r="C39" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="C39" s="2" t="s">
+      <c r="D39" s="2" t="s">
         <v>176</v>
-      </c>
-      <c r="D39" s="2" t="s">
-        <v>177</v>
       </c>
       <c r="E39" s="2">
         <v>2</v>
       </c>
       <c r="F39" s="5" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="G39" s="10"/>
     </row>
     <row r="40" spans="1:7" ht="73.75" x14ac:dyDescent="0.5">
       <c r="A40" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="B40" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="B40" s="2" t="s">
+      <c r="C40" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="C40" s="2" t="s">
+      <c r="D40" s="2" t="s">
         <v>181</v>
-      </c>
-      <c r="D40" s="2" t="s">
-        <v>182</v>
       </c>
       <c r="E40" s="2">
         <v>1</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="G40" s="10"/>
     </row>
     <row r="41" spans="1:7" ht="92.15" x14ac:dyDescent="0.5">
       <c r="A41" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="B41" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="B41" s="2" t="s">
+      <c r="C41" s="2" t="s">
         <v>185</v>
-      </c>
-      <c r="C41" s="2" t="s">
-        <v>186</v>
       </c>
       <c r="D41" s="2"/>
       <c r="E41" s="2">
         <v>1</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="G41" s="10"/>
     </row>
     <row r="42" spans="1:7" ht="55.3" x14ac:dyDescent="0.5">
       <c r="A42" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="B42" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="B42" s="2" t="s">
-        <v>189</v>
-      </c>
       <c r="C42" s="2" t="s">
-        <v>190</v>
+        <v>277</v>
       </c>
       <c r="D42" s="2"/>
       <c r="E42" s="2">
         <v>1</v>
       </c>
-      <c r="F42" s="1" t="s">
-        <v>191</v>
+      <c r="F42" s="5" t="s">
+        <v>189</v>
       </c>
       <c r="G42" s="10"/>
     </row>
     <row r="43" spans="1:7" ht="73.75" x14ac:dyDescent="0.5">
       <c r="A43" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="C43" s="2" t="s">
         <v>192</v>
-      </c>
-      <c r="B43" s="2" t="s">
-        <v>193</v>
-      </c>
-      <c r="C43" s="2" t="s">
-        <v>194</v>
       </c>
       <c r="D43" s="2"/>
       <c r="E43" s="2">
         <v>4</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="G43" s="10"/>
     </row>
     <row r="44" spans="1:7" ht="36.9" x14ac:dyDescent="0.5">
       <c r="A44" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="C44" s="2" t="s">
         <v>196</v>
-      </c>
-      <c r="B44" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="C44" s="2" t="s">
-        <v>198</v>
       </c>
       <c r="D44" s="2"/>
       <c r="E44" s="2">
         <v>1</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="G44" s="10"/>
     </row>
     <row r="45" spans="1:7" ht="36.9" x14ac:dyDescent="0.5">
       <c r="A45" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="C45" s="2" t="s">
         <v>200</v>
-      </c>
-      <c r="B45" s="2" t="s">
-        <v>201</v>
-      </c>
-      <c r="C45" s="2" t="s">
-        <v>202</v>
       </c>
       <c r="D45" s="2"/>
       <c r="E45" s="2">
         <v>10</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="G45" s="10"/>
     </row>
     <row r="46" spans="1:7" ht="36.9" x14ac:dyDescent="0.5">
       <c r="A46" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="C46" s="2" t="s">
         <v>204</v>
-      </c>
-      <c r="B46" s="2" t="s">
-        <v>205</v>
-      </c>
-      <c r="C46" s="2" t="s">
-        <v>206</v>
       </c>
       <c r="D46" s="2"/>
       <c r="E46" s="2">
         <v>4</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="G46" s="11"/>
     </row>
     <row r="47" spans="1:7" ht="55.3" x14ac:dyDescent="0.5">
       <c r="A47" s="6" t="s">
+        <v>206</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="C47" s="2" t="s">
         <v>208</v>
-      </c>
-      <c r="B47" s="2" t="s">
-        <v>209</v>
-      </c>
-      <c r="C47" s="2" t="s">
-        <v>210</v>
       </c>
       <c r="D47" s="7"/>
       <c r="E47" s="2">
         <v>4</v>
       </c>
       <c r="F47" s="6" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="G47" s="11"/>
     </row>
     <row r="48" spans="1:7" ht="36.9" x14ac:dyDescent="0.5">
       <c r="A48" s="6" t="s">
+        <v>210</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="C48" s="2" t="s">
         <v>212</v>
-      </c>
-      <c r="B48" s="2" t="s">
-        <v>213</v>
-      </c>
-      <c r="C48" s="2" t="s">
-        <v>214</v>
       </c>
       <c r="D48" s="7"/>
       <c r="E48" s="2">
         <v>4</v>
       </c>
       <c r="F48" s="6" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="G48" s="11"/>
     </row>
     <row r="49" spans="1:7" ht="36.9" x14ac:dyDescent="0.5">
       <c r="A49" s="6" t="s">
+        <v>214</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="C49" s="2" t="s">
         <v>216</v>
-      </c>
-      <c r="B49" s="2" t="s">
-        <v>217</v>
-      </c>
-      <c r="C49" s="2" t="s">
-        <v>218</v>
       </c>
       <c r="D49" s="7"/>
       <c r="E49" s="2">
         <v>8</v>
       </c>
       <c r="F49" s="6" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="G49" s="11"/>
     </row>
     <row r="50" spans="1:7" ht="36.9" x14ac:dyDescent="0.5">
       <c r="A50" s="8" t="s">
+        <v>218</v>
+      </c>
+      <c r="B50" s="4" t="s">
+        <v>219</v>
+      </c>
+      <c r="C50" s="4" t="s">
         <v>220</v>
-      </c>
-      <c r="B50" s="4" t="s">
-        <v>221</v>
-      </c>
-      <c r="C50" s="4" t="s">
-        <v>222</v>
       </c>
       <c r="D50" s="9"/>
       <c r="E50" s="4">
         <v>4</v>
       </c>
       <c r="F50" s="8" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="G50" s="11"/>
     </row>
     <row r="51" spans="1:7" ht="55.3" x14ac:dyDescent="0.5">
       <c r="A51" s="8" t="s">
+        <v>222</v>
+      </c>
+      <c r="B51" s="4" t="s">
+        <v>223</v>
+      </c>
+      <c r="C51" s="4" t="s">
         <v>224</v>
-      </c>
-      <c r="B51" s="4" t="s">
-        <v>225</v>
-      </c>
-      <c r="C51" s="4" t="s">
-        <v>226</v>
       </c>
       <c r="D51" s="9"/>
       <c r="E51" s="4">
         <v>8</v>
       </c>
       <c r="F51" s="8" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="G51" s="11"/>
     </row>
     <row r="52" spans="1:7" ht="55.3" x14ac:dyDescent="0.5">
       <c r="A52" s="8" t="s">
+        <v>226</v>
+      </c>
+      <c r="B52" s="4" t="s">
+        <v>227</v>
+      </c>
+      <c r="C52" s="4" t="s">
         <v>228</v>
-      </c>
-      <c r="B52" s="4" t="s">
-        <v>229</v>
-      </c>
-      <c r="C52" s="4" t="s">
-        <v>230</v>
       </c>
       <c r="D52" s="9"/>
       <c r="E52" s="4">
         <v>6</v>
       </c>
       <c r="F52" s="8" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="G52" s="11"/>
     </row>
     <row r="53" spans="1:7" ht="55.3" x14ac:dyDescent="0.5">
       <c r="A53" s="8" t="s">
+        <v>230</v>
+      </c>
+      <c r="B53" s="4" t="s">
+        <v>231</v>
+      </c>
+      <c r="C53" s="4" t="s">
         <v>232</v>
-      </c>
-      <c r="B53" s="4" t="s">
-        <v>233</v>
-      </c>
-      <c r="C53" s="4" t="s">
-        <v>234</v>
       </c>
       <c r="D53" s="9"/>
       <c r="E53" s="4">
         <v>2</v>
       </c>
       <c r="F53" s="8" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="G53" s="11"/>
     </row>
     <row r="54" spans="1:7" ht="36.9" x14ac:dyDescent="0.5">
       <c r="A54" s="8" t="s">
+        <v>234</v>
+      </c>
+      <c r="B54" s="4" t="s">
+        <v>235</v>
+      </c>
+      <c r="C54" s="4" t="s">
         <v>236</v>
-      </c>
-      <c r="B54" s="4" t="s">
-        <v>237</v>
-      </c>
-      <c r="C54" s="4" t="s">
-        <v>238</v>
       </c>
       <c r="D54" s="9"/>
       <c r="E54" s="4">
         <v>2</v>
       </c>
       <c r="F54" s="8" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="G54" s="11"/>
     </row>
     <row r="55" spans="1:7" ht="36.9" x14ac:dyDescent="0.5">
       <c r="A55" s="8" t="s">
+        <v>238</v>
+      </c>
+      <c r="B55" s="4" t="s">
+        <v>239</v>
+      </c>
+      <c r="C55" s="4" t="s">
         <v>240</v>
-      </c>
-      <c r="B55" s="4" t="s">
-        <v>241</v>
-      </c>
-      <c r="C55" s="4" t="s">
-        <v>242</v>
       </c>
       <c r="D55" s="9"/>
       <c r="E55" s="4">
         <v>1</v>
       </c>
       <c r="F55" s="8" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="G55" s="11"/>
     </row>
     <row r="56" spans="1:7" ht="55.3" x14ac:dyDescent="0.5">
       <c r="A56" s="8" t="s">
+        <v>242</v>
+      </c>
+      <c r="B56" s="4" t="s">
+        <v>243</v>
+      </c>
+      <c r="C56" s="4" t="s">
         <v>244</v>
-      </c>
-      <c r="B56" s="4" t="s">
-        <v>245</v>
-      </c>
-      <c r="C56" s="4" t="s">
-        <v>246</v>
       </c>
       <c r="D56" s="9"/>
       <c r="E56" s="4">
         <v>1</v>
       </c>
       <c r="F56" s="8" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="G56" s="11"/>
     </row>
     <row r="57" spans="1:7" ht="55.3" x14ac:dyDescent="0.5">
       <c r="A57" s="8" t="s">
+        <v>246</v>
+      </c>
+      <c r="B57" s="4" t="s">
+        <v>247</v>
+      </c>
+      <c r="C57" s="4" t="s">
         <v>248</v>
-      </c>
-      <c r="B57" s="4" t="s">
-        <v>249</v>
-      </c>
-      <c r="C57" s="4" t="s">
-        <v>250</v>
       </c>
       <c r="D57" s="9"/>
       <c r="E57" s="4">
         <v>4</v>
       </c>
       <c r="F57" s="8" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="G57" s="11"/>
     </row>
     <row r="58" spans="1:7" ht="55.3" x14ac:dyDescent="0.5">
       <c r="A58" s="8" t="s">
+        <v>250</v>
+      </c>
+      <c r="B58" s="4" t="s">
+        <v>251</v>
+      </c>
+      <c r="C58" s="4" t="s">
         <v>252</v>
-      </c>
-      <c r="B58" s="4" t="s">
-        <v>253</v>
-      </c>
-      <c r="C58" s="4" t="s">
-        <v>254</v>
       </c>
       <c r="D58" s="9"/>
       <c r="E58" s="4">
         <v>2</v>
       </c>
       <c r="F58" s="8" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="G58" s="11"/>
     </row>
     <row r="59" spans="1:7" ht="55.3" x14ac:dyDescent="0.5">
       <c r="A59" s="8" t="s">
-        <v>256</v>
-      </c>
-      <c r="B59" s="4">
-        <v>60311002111526</v>
+        <v>254</v>
+      </c>
+      <c r="B59" s="4" t="s">
+        <v>276</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="D59" s="9"/>
       <c r="E59" s="4">
         <v>4</v>
       </c>
-      <c r="F59" s="8" t="s">
-        <v>258</v>
+      <c r="F59" s="24" t="s">
+        <v>256</v>
       </c>
       <c r="G59" s="11"/>
     </row>
     <row r="60" spans="1:7" ht="73.75" x14ac:dyDescent="0.5">
       <c r="A60" s="8" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B60" s="4">
         <v>2453690000</v>
       </c>
       <c r="C60" s="4" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="D60" s="9"/>
       <c r="E60" s="4">
         <v>1</v>
       </c>
       <c r="F60" s="8" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="G60" s="11"/>
     </row>
     <row r="61" spans="1:7" ht="55.3" x14ac:dyDescent="0.5">
       <c r="A61" s="8" t="s">
+        <v>260</v>
+      </c>
+      <c r="B61" s="4" t="s">
+        <v>261</v>
+      </c>
+      <c r="C61" s="4" t="s">
         <v>262</v>
-      </c>
-      <c r="B61" s="4" t="s">
-        <v>263</v>
-      </c>
-      <c r="C61" s="4" t="s">
-        <v>264</v>
       </c>
       <c r="D61" s="9"/>
       <c r="E61" s="4">
         <v>4</v>
       </c>
       <c r="F61" s="8" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="G61" s="11"/>
     </row>
     <row r="62" spans="1:7" ht="36.9" x14ac:dyDescent="0.5">
       <c r="A62" s="8" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="B62" s="4">
         <v>7461098</v>
       </c>
       <c r="C62" s="4" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="D62" s="9"/>
       <c r="E62" s="4">
         <v>2</v>
       </c>
       <c r="F62" s="8" t="s">
+        <v>266</v>
+      </c>
+      <c r="G62" s="11"/>
+    </row>
+    <row r="63" spans="1:7" ht="55.3" x14ac:dyDescent="0.5">
+      <c r="A63" s="20" t="s">
+        <v>267</v>
+      </c>
+      <c r="B63" s="4" t="s">
         <v>268</v>
       </c>
-      <c r="G62" s="11"/>
-    </row>
-    <row r="63" spans="1:7" ht="55.3" x14ac:dyDescent="0.5">
-      <c r="A63" s="17" t="s">
+      <c r="C63" s="4" t="s">
         <v>269</v>
       </c>
-      <c r="B63" s="13" t="s">
+      <c r="D63" s="9"/>
+      <c r="E63" s="4">
+        <v>2</v>
+      </c>
+      <c r="F63" s="8" t="s">
         <v>270</v>
       </c>
-      <c r="C63" s="13" t="s">
+    </row>
+    <row r="64" spans="1:7" ht="55.75" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A64" s="21" t="s">
         <v>271</v>
       </c>
-      <c r="D63" s="14"/>
-      <c r="E63" s="13">
-        <v>2</v>
-      </c>
-      <c r="F63" s="12" t="s">
+      <c r="B64" s="22" t="s">
         <v>272</v>
       </c>
-    </row>
-    <row r="64" spans="1:7" ht="55.75" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A64" s="18" t="s">
+      <c r="C64" s="22" t="s">
         <v>273</v>
       </c>
-      <c r="B64" s="19" t="s">
+      <c r="D64" s="23"/>
+      <c r="E64" s="22">
+        <v>1</v>
+      </c>
+      <c r="F64" s="21" t="s">
         <v>274</v>
-      </c>
-      <c r="C64" s="19" t="s">
-        <v>275</v>
-      </c>
-      <c r="D64" s="20"/>
-      <c r="E64" s="19">
-        <v>1</v>
-      </c>
-      <c r="F64" s="18" t="s">
-        <v>276</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="F23" r:id="rId1" xr:uid="{D6AC9AED-CE86-4F0C-A339-B86E7AE3973E}"/>
+    <hyperlink ref="F9" r:id="rId2" xr:uid="{B4EC195F-9D17-4B9C-92BF-54C8B826CDAD}"/>
+    <hyperlink ref="F59" r:id="rId3" xr:uid="{200DA76B-A092-4D2F-823A-72314EC416BF}"/>
+    <hyperlink ref="F42" r:id="rId4" xr:uid="{7E9CA9B5-041D-4A86-8028-ADB8E605EDB2}"/>
+    <hyperlink ref="F14" r:id="rId5" xr:uid="{2E5D91BE-104C-4C78-9BFE-3B5E689A07F3}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId6"/>
 </worksheet>
 </file>
 

</xml_diff>